<commit_message>
Upload and clean environment
</commit_message>
<xml_diff>
--- a/Docs/DesignContent/DataSpec/DataDictionary.xlsx
+++ b/Docs/DesignContent/DataSpec/DataDictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="2160" windowHeight="1110" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="2160" windowHeight="1170" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="230">
   <si>
     <t>contact.docx</t>
   </si>
@@ -1437,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,19 +2221,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -2246,8 +2247,11 @@
       <c r="D1" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2260,8 +2264,11 @@
       <c r="D3" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2274,8 +2281,11 @@
       <c r="D4" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2288,8 +2298,11 @@
       <c r="D5" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -2302,59 +2315,80 @@
       <c r="D6" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>117</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>90</v>
       </c>

</xml_diff>